<commit_message>
add AMR scripts and meta data files
</commit_message>
<xml_diff>
--- a/06. Meta data/zenodo url file.xlsx
+++ b/06. Meta data/zenodo url file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\HOLIFOOD\06. Meta data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\DATAWFSR-CHEFS\CHEFS\06. Meta data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6AFA9C-C467-4CB2-84A1-3BC6B072B316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D513199-E608-4C90-BC1B-E18DAA15EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{613B4D81-A68D-43B4-8DEE-F304873255D0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{613B4D81-A68D-43B4-8DEE-F304873255D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="333">
   <si>
     <t>Country</t>
   </si>
@@ -733,12 +733,6 @@
     <t>https://zenodo.org/records/10531795</t>
   </si>
   <si>
-    <t>2021b</t>
-  </si>
-  <si>
-    <t>2021a</t>
-  </si>
-  <si>
     <t>https://zenodo.org/records/4557797</t>
   </si>
   <si>
@@ -947,6 +941,102 @@
   </si>
   <si>
     <t>https://zenodo.org/records/10534523</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14718767</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713717</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720296</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14718483</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14717630</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713363</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713093</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720337</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713433</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713283</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713657</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14717885</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720131</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14718525</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720203</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14719738</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14718670</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14712883</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713540</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14718438</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713603</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720260</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720169</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720240</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14720522</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14718840</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713134</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14724207</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14717812</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14718713</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14717953</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/14713481</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1910,7 @@
         <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C31" t="s">
         <v>140</v>
@@ -1915,7 +2005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88DF733-2407-4CFB-9F47-0DD7EAF6A6E3}">
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -1931,7 +2021,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.5">
@@ -1956,7 +2046,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.5">
@@ -2119,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D6D02A-B16E-43F4-8AD2-599F781335B8}">
-  <dimension ref="A1:C128"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A128" sqref="A2:A128"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
@@ -2188,13 +2278,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>173</v>
+        <v>112</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="C6">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
@@ -2202,10 +2292,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
@@ -2213,10 +2303,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
@@ -2224,32 +2314,32 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C10">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>180</v>
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="C11">
-        <v>2019</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
@@ -2257,10 +2347,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C12">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
@@ -2268,43 +2358,43 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C14">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C15">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>185</v>
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="C16">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
@@ -2312,172 +2402,172 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C17">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C18">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>188</v>
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>185</v>
       </c>
       <c r="C19">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C20">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>190</v>
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="C21">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C22">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>192</v>
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="C23">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C24">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C25">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>195</v>
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="C26">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C27">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C28">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C30">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>200</v>
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="C31">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C32">
         <v>2022</v>
@@ -2485,21 +2575,21 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C33">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C34">
         <v>2019</v>
@@ -2507,32 +2597,32 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C35">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" t="s">
-        <v>205</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="C36">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>206</v>
+        <v>39</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="C37">
         <v>2019</v>
@@ -2540,10 +2630,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C38">
         <v>2021</v>
@@ -2551,10 +2641,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C39">
         <v>2022</v>
@@ -2562,43 +2652,43 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" t="s">
-        <v>209</v>
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="C40">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C41">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C42">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C43">
         <v>2021</v>
@@ -2606,10 +2696,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C44">
         <v>2022</v>
@@ -2617,87 +2707,87 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" t="s">
-        <v>214</v>
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C46">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C47">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C48">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C49">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" t="s">
-        <v>219</v>
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="C50">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C51">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C52">
         <v>2020</v>
@@ -2705,21 +2795,21 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C54">
         <v>2022</v>
@@ -2727,32 +2817,32 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" t="s">
-        <v>224</v>
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="C55">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C56">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -2760,109 +2850,109 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C58">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C59">
-        <v>2022</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
-        <v>117</v>
-      </c>
-      <c r="B60" t="s">
-        <v>229</v>
-      </c>
-      <c r="C60" t="s">
-        <v>232</v>
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C60">
+        <v>2023</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" t="s">
-        <v>230</v>
-      </c>
-      <c r="C61" t="s">
-        <v>231</v>
+        <v>64</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C61">
+        <v>2019</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C62">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C63">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C64">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" t="s">
-        <v>236</v>
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="C65">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="C66">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C67">
         <v>2022</v>
@@ -2870,10 +2960,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="C68">
         <v>2021</v>
@@ -2881,76 +2971,76 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C69">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>88</v>
-      </c>
-      <c r="B70" t="s">
-        <v>241</v>
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="C70">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71" t="s">
-        <v>242</v>
+        <v>74</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="C71">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="C72">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C73">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>93</v>
-      </c>
-      <c r="B74" t="s">
-        <v>245</v>
+        <v>74</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="C74">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>93</v>
-      </c>
-      <c r="B75" t="s">
-        <v>246</v>
+        <v>117</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="C75">
         <v>2020</v>
@@ -2958,120 +3048,120 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="B76" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="C76">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
-        <v>93</v>
-      </c>
-      <c r="B77" t="s">
-        <v>248</v>
+        <v>117</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="C77">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>98</v>
-      </c>
-      <c r="B78" t="s">
-        <v>249</v>
+        <v>79</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="C78">
-        <v>2022</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="C79">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="C80">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="C81">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
-        <v>103</v>
-      </c>
-      <c r="B82" t="s">
-        <v>253</v>
+        <v>79</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="C82">
-        <v>2019</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="C83">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="C84">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="C85">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="C86">
         <v>2020</v>
@@ -3079,87 +3169,87 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A87" t="s">
-        <v>121</v>
-      </c>
-      <c r="B87" t="s">
-        <v>258</v>
+        <v>83</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="C87">
-        <v>2019</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
-        <v>121</v>
-      </c>
-      <c r="B88" t="s">
-        <v>259</v>
+        <v>88</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="C88">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="C89">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A90" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="C90">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="C91">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A92" t="s">
-        <v>125</v>
-      </c>
-      <c r="B92" t="s">
-        <v>263</v>
+        <v>88</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="C92">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A93" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="C93">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A94" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C94">
         <v>2020</v>
@@ -3167,21 +3257,21 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C95">
-        <v>2022</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A96" t="s">
-        <v>129</v>
-      </c>
-      <c r="B96" t="s">
-        <v>267</v>
+        <v>93</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="C96">
         <v>2021</v>
@@ -3189,21 +3279,21 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A97" t="s">
-        <v>129</v>
-      </c>
-      <c r="B97" t="s">
-        <v>268</v>
+        <v>93</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="C97">
-        <v>2019</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A98" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="C98">
         <v>2022</v>
@@ -3211,10 +3301,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A99" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="C99">
         <v>2020</v>
@@ -3222,208 +3312,208 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C100">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A101" t="s">
-        <v>134</v>
-      </c>
-      <c r="B101" t="s">
-        <v>272</v>
+        <v>98</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="C101">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A102" t="s">
-        <v>139</v>
-      </c>
-      <c r="B102" t="s">
-        <v>274</v>
+        <v>98</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="C102">
-        <v>2019</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A103" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="C103">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A104" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="C104">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A105" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="C105">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A106" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="C106">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A107" t="s">
-        <v>145</v>
-      </c>
-      <c r="B107" t="s">
-        <v>279</v>
+        <v>103</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="C107">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A108" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="B108" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="C108">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A109" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="B109" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="C109">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="B110" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="C110">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A111" t="s">
-        <v>149</v>
-      </c>
-      <c r="B111" t="s">
-        <v>283</v>
+        <v>121</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="C111">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A112" t="s">
-        <v>149</v>
-      </c>
-      <c r="B112" t="s">
-        <v>284</v>
+        <v>121</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="C112">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A113" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="B113" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="C113">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A114" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="B114" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="C114">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A115" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="B115" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="C115">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A116" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="B116" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="C116">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A117" t="s">
-        <v>154</v>
-      </c>
-      <c r="B117" t="s">
-        <v>289</v>
+        <v>125</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="C117">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A118" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="B118" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="C118">
         <v>2020</v>
@@ -3431,32 +3521,32 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A119" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="B119" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="C119">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A120" t="s">
-        <v>292</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>293</v>
+        <v>129</v>
+      </c>
+      <c r="B120" t="s">
+        <v>265</v>
       </c>
       <c r="C120">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A121" t="s">
-        <v>292</v>
+        <v>129</v>
       </c>
       <c r="B121" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="C121">
         <v>2019</v>
@@ -3464,54 +3554,54 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A122" t="s">
-        <v>292</v>
-      </c>
-      <c r="B122" t="s">
-        <v>295</v>
+        <v>129</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="C122">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A123" t="s">
-        <v>296</v>
+        <v>134</v>
       </c>
       <c r="B123" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="C123">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A124" t="s">
-        <v>296</v>
+        <v>134</v>
       </c>
       <c r="B124" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="C124">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A125" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B125" t="s">
-        <v>299</v>
+        <v>269</v>
       </c>
       <c r="C125">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A126" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B126" t="s">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="C126">
         <v>2019</v>
@@ -3519,24 +3609,376 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A127" t="s">
-        <v>25</v>
-      </c>
-      <c r="B127" t="s">
-        <v>301</v>
+        <v>134</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="C127">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A128" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" t="s">
+        <v>272</v>
+      </c>
+      <c r="C128">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A129" t="s">
+        <v>139</v>
+      </c>
+      <c r="B129" t="s">
+        <v>273</v>
+      </c>
+      <c r="C129">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A130" t="s">
+        <v>139</v>
+      </c>
+      <c r="B130" t="s">
+        <v>274</v>
+      </c>
+      <c r="C130">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A131" t="s">
+        <v>139</v>
+      </c>
+      <c r="B131" t="s">
+        <v>275</v>
+      </c>
+      <c r="C131">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A132" t="s">
+        <v>139</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C132">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A133" t="s">
+        <v>145</v>
+      </c>
+      <c r="B133" t="s">
+        <v>276</v>
+      </c>
+      <c r="C133">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A134" t="s">
+        <v>145</v>
+      </c>
+      <c r="B134" t="s">
+        <v>277</v>
+      </c>
+      <c r="C134">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A135" t="s">
+        <v>145</v>
+      </c>
+      <c r="B135" t="s">
+        <v>278</v>
+      </c>
+      <c r="C135">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A136" t="s">
+        <v>145</v>
+      </c>
+      <c r="B136" t="s">
+        <v>279</v>
+      </c>
+      <c r="C136">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A137" t="s">
+        <v>145</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C137">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A138" t="s">
+        <v>149</v>
+      </c>
+      <c r="B138" t="s">
+        <v>280</v>
+      </c>
+      <c r="C138">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A139" t="s">
+        <v>149</v>
+      </c>
+      <c r="B139" t="s">
+        <v>281</v>
+      </c>
+      <c r="C139">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A140" t="s">
+        <v>149</v>
+      </c>
+      <c r="B140" t="s">
+        <v>282</v>
+      </c>
+      <c r="C140">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A141" t="s">
+        <v>149</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C141">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A142" t="s">
+        <v>149</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C142">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A143" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" t="s">
+        <v>284</v>
+      </c>
+      <c r="C143">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A144" t="s">
+        <v>154</v>
+      </c>
+      <c r="B144" t="s">
+        <v>285</v>
+      </c>
+      <c r="C144">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A145" t="s">
+        <v>154</v>
+      </c>
+      <c r="B145" t="s">
+        <v>286</v>
+      </c>
+      <c r="C145">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A146" t="s">
+        <v>154</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C146">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A147" t="s">
+        <v>154</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C147">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A148" t="s">
+        <v>159</v>
+      </c>
+      <c r="B148" t="s">
+        <v>288</v>
+      </c>
+      <c r="C148">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A149" t="s">
+        <v>159</v>
+      </c>
+      <c r="B149" t="s">
+        <v>289</v>
+      </c>
+      <c r="C149">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A150" t="s">
+        <v>290</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C150">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A151" t="s">
+        <v>290</v>
+      </c>
+      <c r="B151" t="s">
+        <v>292</v>
+      </c>
+      <c r="C151">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A152" t="s">
+        <v>290</v>
+      </c>
+      <c r="B152" t="s">
+        <v>293</v>
+      </c>
+      <c r="C152">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A153" t="s">
+        <v>290</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C153">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A154" t="s">
+        <v>294</v>
+      </c>
+      <c r="B154" t="s">
+        <v>295</v>
+      </c>
+      <c r="C154">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A155" t="s">
+        <v>294</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C155">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A156" t="s">
         <v>25</v>
       </c>
-      <c r="B128" t="s">
-        <v>302</v>
-      </c>
-      <c r="C128">
+      <c r="B156" t="s">
+        <v>297</v>
+      </c>
+      <c r="C156">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A157" t="s">
+        <v>25</v>
+      </c>
+      <c r="B157" t="s">
+        <v>298</v>
+      </c>
+      <c r="C157">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A158" t="s">
+        <v>25</v>
+      </c>
+      <c r="B158" t="s">
+        <v>299</v>
+      </c>
+      <c r="C158">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A159" t="s">
+        <v>25</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C159">
         <v>2022</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A160" t="s">
+        <v>25</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C160">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>
@@ -3545,8 +3987,53 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{47A63E53-1E6F-41DD-9B48-1EF27845452C}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{FCB32D86-7076-4E11-A554-0337CA5C2101}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{3E2E455F-BAC6-4729-98CB-156A41147250}"/>
-    <hyperlink ref="B19" r:id="rId5" xr:uid="{E7A205EB-267E-4D1C-903A-015D933E8778}"/>
-    <hyperlink ref="B120" r:id="rId6" xr:uid="{4B1F20B3-89F8-44E3-9FB9-00BDEE0ACCAC}"/>
+    <hyperlink ref="B23" r:id="rId5" xr:uid="{E7A205EB-267E-4D1C-903A-015D933E8778}"/>
+    <hyperlink ref="B150" r:id="rId6" xr:uid="{4B1F20B3-89F8-44E3-9FB9-00BDEE0ACCAC}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{0F4E4DD3-3373-4729-848E-D78B67C0F916}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{048437C1-B340-445B-8A18-62151816414D}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{25307ACD-4D16-4CE8-B4B8-75F4242B444D}"/>
+    <hyperlink ref="B21" r:id="rId10" xr:uid="{63EE918F-6CD7-4935-9524-A18F522DE730}"/>
+    <hyperlink ref="B26" r:id="rId11" xr:uid="{2D3D3EDA-6AFC-411F-8CD8-C19D4B71868F}"/>
+    <hyperlink ref="B31" r:id="rId12" xr:uid="{36CCC21A-85CC-41A9-B44C-80F317BF4266}"/>
+    <hyperlink ref="B36" r:id="rId13" xr:uid="{B8E047D3-A42B-49E8-953A-5A3E076DBE74}"/>
+    <hyperlink ref="B37" r:id="rId14" xr:uid="{619D7AE4-8182-45F6-873A-02749DA3B125}"/>
+    <hyperlink ref="B40" r:id="rId15" xr:uid="{06B2664F-38F0-4B94-AE77-E83322B75CD4}"/>
+    <hyperlink ref="B45" r:id="rId16" xr:uid="{5132079A-6ED3-4121-842E-7C1C49F79B6C}"/>
+    <hyperlink ref="B50" r:id="rId17" xr:uid="{41680ED7-E369-4C19-A6FE-863AAC783237}"/>
+    <hyperlink ref="B55" r:id="rId18" xr:uid="{73C81868-3924-4AB4-B8E5-55CE4C3B2CED}"/>
+    <hyperlink ref="B60" r:id="rId19" xr:uid="{9A467919-BE66-41A3-BF56-DBA2124FD95D}"/>
+    <hyperlink ref="B61" r:id="rId20" xr:uid="{6ED7D957-C02E-4AF8-BBAF-8F047851F7C3}"/>
+    <hyperlink ref="B65" r:id="rId21" xr:uid="{4D11B6EF-A9DF-4668-AA00-7A1CD927C8BD}"/>
+    <hyperlink ref="B70" r:id="rId22" xr:uid="{6EF4742B-1718-4E04-9860-F4DBE7169024}"/>
+    <hyperlink ref="B71" r:id="rId23" xr:uid="{CD1C6889-9911-4042-8C8D-0A44AA228E1E}"/>
+    <hyperlink ref="B74" r:id="rId24" xr:uid="{0DB10CB6-6E5C-4652-9F07-9A5533033910}"/>
+    <hyperlink ref="B75" r:id="rId25" xr:uid="{0489A3E1-28D9-461D-870E-F22F0B311F01}"/>
+    <hyperlink ref="B77" r:id="rId26" xr:uid="{851BA6CD-5409-4AF1-B738-969037D31D2A}"/>
+    <hyperlink ref="B78" r:id="rId27" xr:uid="{A5B13220-3C8F-4011-905A-A3C42C93834B}"/>
+    <hyperlink ref="B82" r:id="rId28" xr:uid="{744678C9-F5B3-416D-AFA0-EB842FAA2083}"/>
+    <hyperlink ref="B87" r:id="rId29" xr:uid="{2ED72EB8-90FE-491A-9581-515A6C51CBA3}"/>
+    <hyperlink ref="B88" r:id="rId30" xr:uid="{31DBB899-7372-487E-B4E8-31D69B07F8FA}"/>
+    <hyperlink ref="B92" r:id="rId31" xr:uid="{C7931B0B-39A7-446A-ADCF-AE5E03EEE7DD}"/>
+    <hyperlink ref="B96" r:id="rId32" xr:uid="{E599C0DC-E452-4B69-9432-E7515A2AB652}"/>
+    <hyperlink ref="B97" r:id="rId33" xr:uid="{65EF114F-1E30-42C0-8FB2-BED3438F09E1}"/>
+    <hyperlink ref="B101" r:id="rId34" xr:uid="{E51F1406-05C0-460A-8E2B-DF5272FE3E69}"/>
+    <hyperlink ref="B102" r:id="rId35" xr:uid="{D8F206DE-E657-4BB8-9273-9EE694AF6392}"/>
+    <hyperlink ref="B107" r:id="rId36" xr:uid="{B02E760E-D91E-4C9B-B426-499CE978C3E2}"/>
+    <hyperlink ref="B111" r:id="rId37" xr:uid="{E06B1DA7-59D5-43A0-BB17-8715120029CC}"/>
+    <hyperlink ref="B112" r:id="rId38" xr:uid="{43791D2E-2B9D-4E7C-95C0-509B12790376}"/>
+    <hyperlink ref="B117" r:id="rId39" xr:uid="{425CE522-1AC1-4FFB-A1BA-DCEFE59997BD}"/>
+    <hyperlink ref="B122" r:id="rId40" xr:uid="{98D248F5-F491-42FC-A8AD-FA57D6B7D206}"/>
+    <hyperlink ref="B127" r:id="rId41" xr:uid="{F91BCD5F-CB1B-42F7-839E-E0158852C058}"/>
+    <hyperlink ref="B132" r:id="rId42" xr:uid="{6E5FFD1E-4D78-4AC9-BA1E-C9040681D885}"/>
+    <hyperlink ref="B137" r:id="rId43" xr:uid="{DD94404A-97B8-4B1D-9313-E4B889003B1E}"/>
+    <hyperlink ref="B141" r:id="rId44" xr:uid="{BFF7A041-D0F2-4275-B623-B656EB431B7E}"/>
+    <hyperlink ref="B142" r:id="rId45" xr:uid="{A0DD10D1-1147-4D9F-8B66-5330D509F842}"/>
+    <hyperlink ref="B146" r:id="rId46" xr:uid="{ED53DD64-2D7B-408F-A293-FF70FD391E59}"/>
+    <hyperlink ref="B147" r:id="rId47" xr:uid="{492F6648-7A1B-49D0-A014-333456B150D6}"/>
+    <hyperlink ref="B153" r:id="rId48" xr:uid="{4674F6FF-008A-4808-9F27-9636727F0DF3}"/>
+    <hyperlink ref="B155" r:id="rId49" xr:uid="{D7A39616-2BFE-46AE-BC65-1820ACF2581B}"/>
+    <hyperlink ref="B159" r:id="rId50" xr:uid="{3D827A6E-FFCD-44A4-8A9C-C26464F20850}"/>
+    <hyperlink ref="B160" r:id="rId51" xr:uid="{3637F5E1-17CF-4D25-8877-08E6AB4ABB8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
improvements suggested by Rosan
</commit_message>
<xml_diff>
--- a/06. Meta data/zenodo url file.xlsx
+++ b/06. Meta data/zenodo url file.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\DATAWFSR-CHEFS\CHEFS\06. Meta data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\CHEFS Datascience\CHEFS\06. Meta data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D513199-E608-4C90-BC1B-E18DAA15EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4260FCD9-D33D-4C7B-BA74-0DCB43C94B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{613B4D81-A68D-43B4-8DEE-F304873255D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="countries" sheetId="3" r:id="rId2"/>
-    <sheet name="microbiological" sheetId="2" r:id="rId3"/>
+    <sheet name="microbiological-AMR" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>